<commit_message>
docs: 📝 made some research
</commit_message>
<xml_diff>
--- a/doc/journal_de_travail.xlsx
+++ b/doc/journal_de_travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TB\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B569FF66-61E2-4D47-9269-E3235E667462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030B273F-06D8-4D7B-A5F2-799FDBA084D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -49,13 +49,25 @@
     <t>Quoi</t>
   </si>
   <si>
-    <t>Cahier des charges</t>
-  </si>
-  <si>
     <t>Durée</t>
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Analyse et état de l'art</t>
+  </si>
+  <si>
+    <t>Réalisation du modèle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réalisation de l'application </t>
+  </si>
+  <si>
+    <t>Tests et validations</t>
+  </si>
+  <si>
+    <t>Gestion du projet, documentation et présentation</t>
   </si>
 </sst>
 </file>
@@ -381,7 +393,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -389,7 +401,8 @@
     <col min="1" max="1" width="13.140625" style="2" customWidth="1"/>
     <col min="2" max="3" width="11.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="44.140625" customWidth="1"/>
+    <col min="5" max="5" width="46" customWidth="1"/>
+    <col min="8" max="8" width="45.28515625" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -404,7 +417,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -425,14 +438,14 @@
         <v>0.16666666666666669</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I2" s="1">
         <f>SUM(D2:D37)</f>
-        <v>-2.0833333333333315E-2</v>
+        <v>0.68680555555555567</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -450,7 +463,7 @@
         <v>0.16666666666666669</v>
       </c>
       <c r="E3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -468,7 +481,10 @@
         <v>4.166666666666663E-2</v>
       </c>
       <c r="E4" t="s">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -478,15 +494,36 @@
       <c r="B5" s="1">
         <v>0.39583333333333331</v>
       </c>
+      <c r="C5" s="1">
+        <v>0.41944444444444445</v>
+      </c>
       <c r="D5" s="1">
         <f t="shared" si="0"/>
-        <v>-0.39583333333333331</v>
+        <v>2.3611111111111138E-2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>45474</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.28819444444444448</v>
+      </c>
+      <c r="H6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -494,12 +531,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="H7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D8" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="H8" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D9" s="1">
@@ -676,6 +719,11 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{88B0857C-B8C6-49F2-B590-DD6F017D3688}">
+      <formula1>$H$4:$H$8</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
docs: 📝 wrote model research
</commit_message>
<xml_diff>
--- a/doc/journal_de_travail.xlsx
+++ b/doc/journal_de_travail.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TB\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030B273F-06D8-4D7B-A5F2-799FDBA084D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9DABC9-D36D-4E52-87FF-AD27E6CA87DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="2190" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Journal" sheetId="1" r:id="rId1"/>
+    <sheet name="Utils" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -393,7 +394,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,7 +403,7 @@
     <col min="2" max="3" width="11.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" customWidth="1"/>
     <col min="5" max="5" width="46" customWidth="1"/>
-    <col min="8" max="8" width="45.28515625" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -445,7 +446,7 @@
       </c>
       <c r="I2" s="1">
         <f>SUM(D2:D37)</f>
-        <v>0.68680555555555567</v>
+        <v>0.94791666666666685</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -483,9 +484,6 @@
       <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="H4" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -504,9 +502,6 @@
       <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="H5" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -522,17 +517,20 @@
         <f t="shared" si="0"/>
         <v>0.28819444444444448</v>
       </c>
-      <c r="H6" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>45475</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.63611111111111118</v>
+      </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H7" t="s">
-        <v>9</v>
+        <v>0.26111111111111118</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -540,9 +538,6 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D9" s="1">
@@ -719,11 +714,61 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{88B0857C-B8C6-49F2-B590-DD6F017D3688}">
-      <formula1>$H$4:$H$8</formula1>
-    </dataValidation>
-  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{88B0857C-B8C6-49F2-B590-DD6F017D3688}">
+          <x14:formula1>
+            <xm:f>Utils!$B$2:$B$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>E1:E1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{439C75DC-391B-42D8-BD8F-042837A29DC7}">
+  <dimension ref="B2:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="45.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
docs: 📝 added pros and cons for CNN models
</commit_message>
<xml_diff>
--- a/doc/journal_de_travail.xlsx
+++ b/doc/journal_de_travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TB\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9DABC9-D36D-4E52-87FF-AD27E6CA87DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73B95D7-3781-4AF5-BD2F-23E70881520D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5760" yWindow="2190" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -394,7 +394,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +446,7 @@
       </c>
       <c r="I2" s="1">
         <f>SUM(D2:D37)</f>
-        <v>0.94791666666666685</v>
+        <v>1.0937500000000002</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -517,6 +517,9 @@
         <f t="shared" si="0"/>
         <v>0.28819444444444448</v>
       </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -532,17 +535,44 @@
         <f t="shared" si="0"/>
         <v>0.26111111111111118</v>
       </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>45475</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.80555555555555547</v>
+      </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>45476</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.52083333333333337</v>
+      </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.10416666666666669</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
docs: 📝 added research limitation
</commit_message>
<xml_diff>
--- a/doc/journal_de_travail.xlsx
+++ b/doc/journal_de_travail.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TB\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73B95D7-3781-4AF5-BD2F-23E70881520D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D892068-E9D7-43E5-8F2D-87E0DA1F59E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="2190" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3810" yWindow="1800" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
     <sheet name="Utils" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -394,7 +395,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +447,7 @@
       </c>
       <c r="I2" s="1">
         <f>SUM(D2:D37)</f>
-        <v>1.0937500000000002</v>
+        <v>1.2604166666666667</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -576,9 +577,21 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>45478</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.74305555555555547</v>
+      </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.16666666666666652</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
docs: 📝 added datasets and architecture
</commit_message>
<xml_diff>
--- a/doc/journal_de_travail.xlsx
+++ b/doc/journal_de_travail.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TB\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46A418B-0753-45B2-AEDF-FC9B7FD60C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F8DC84-9C03-44B3-AFF7-7C8AA1C1F8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -107,10 +107,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,7 +395,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,9 +445,9 @@
       <c r="H2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="3">
         <f>SUM(D2:D37)</f>
-        <v>1.40625</v>
+        <v>1.7930555555555556</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -612,15 +613,39 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>45482</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.76180555555555562</v>
+      </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.3173611111111112</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>45482</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.90277777777777779</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.944444444444442E-2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -769,6 +794,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">

</xml_diff>

<commit_message>
docs:📝 finished AI part
</commit_message>
<xml_diff>
--- a/doc/journal_de_travail.xlsx
+++ b/doc/journal_de_travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TB\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F8DC84-9C03-44B3-AFF7-7C8AA1C1F8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF836C0-CD35-4557-89F0-4FDE65F956DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -395,7 +395,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,7 +404,7 @@
     <col min="2" max="3" width="11.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" customWidth="1"/>
     <col min="5" max="5" width="46" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="44.85546875" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -424,6 +424,13 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3">
+        <f>SUMIF(E:E, H1, D:D)</f>
+        <v>1.5222222222222221</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
@@ -443,11 +450,11 @@
         <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I2" s="3">
-        <f>SUM(D2:D37)</f>
-        <v>1.7930555555555556</v>
+        <f t="shared" ref="I2:I5" si="0">SUMIF(E:E, H2, D:D)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -461,11 +468,18 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D37" si="0">C3-B3</f>
+        <f t="shared" ref="D3:D37" si="1">C3-B3</f>
         <v>0.16666666666666669</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -479,11 +493,18 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -497,11 +518,18 @@
         <v>0.41944444444444445</v>
       </c>
       <c r="D5" s="1">
+        <f t="shared" si="1"/>
+        <v>2.3611111111111138E-2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="3">
         <f t="shared" si="0"/>
-        <v>2.3611111111111138E-2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -515,7 +543,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.28819444444444448</v>
       </c>
       <c r="E6" t="s">
@@ -533,11 +561,18 @@
         <v>0.63611111111111118</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.26111111111111118</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="3">
+        <f>SUM(I1:I5)</f>
+        <v>1.8972222222222221</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -551,7 +586,7 @@
         <v>0.80555555555555547</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="E8" t="s">
@@ -569,7 +604,7 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.10416666666666669</v>
       </c>
       <c r="E9" t="s">
@@ -587,7 +622,7 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.16666666666666652</v>
       </c>
       <c r="E10" t="s">
@@ -605,7 +640,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.14583333333333326</v>
       </c>
       <c r="E11" t="s">
@@ -623,7 +658,7 @@
         <v>0.76180555555555562</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.3173611111111112</v>
       </c>
       <c r="E12" t="s">
@@ -641,7 +676,7 @@
         <v>0.97222222222222221</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.944444444444442E-2</v>
       </c>
       <c r="E13" t="s">
@@ -649,146 +684,158 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>45483</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.49305555555555558</v>
+      </c>
       <c r="D14" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.10416666666666669</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D28" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D29" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D30" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D31" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D32" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -815,7 +862,7 @@
   <dimension ref="B2:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
feat: ✨ added working-ish prototype
</commit_message>
<xml_diff>
--- a/doc/journal_de_travail.xlsx
+++ b/doc/journal_de_travail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TB\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF836C0-CD35-4557-89F0-4FDE65F956DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2EDB374-A35B-416E-931D-593E4BBD1FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4065" yWindow="3030" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -395,7 +395,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,7 +429,7 @@
       </c>
       <c r="I1" s="3">
         <f>SUMIF(E:E, H1, D:D)</f>
-        <v>1.5222222222222221</v>
+        <v>1.8138888888888889</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -572,7 +572,7 @@
       </c>
       <c r="I7" s="3">
         <f>SUM(I1:I5)</f>
-        <v>1.8972222222222221</v>
+        <v>2.1888888888888891</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -702,9 +702,21 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>45483</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.83333333333333337</v>
+      </c>
       <c r="D15" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.29166666666666674</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
docs: 📝 added model library choice + prototype ffi
</commit_message>
<xml_diff>
--- a/doc/journal_de_travail.xlsx
+++ b/doc/journal_de_travail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TB\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2EDB374-A35B-416E-931D-593E4BBD1FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0539EA3-219D-40BB-8D6E-24F6BAA17A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4065" yWindow="3030" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -395,7 +395,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,7 +429,7 @@
       </c>
       <c r="I1" s="3">
         <f>SUMIF(E:E, H1, D:D)</f>
-        <v>1.8138888888888889</v>
+        <v>2.5951388888888891</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -572,7 +572,7 @@
       </c>
       <c r="I7" s="3">
         <f>SUM(I1:I5)</f>
-        <v>2.1888888888888891</v>
+        <v>2.9701388888888891</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -720,102 +720,138 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>45484</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.55555555555555558</v>
+      </c>
       <c r="D16" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+        <v>0.18055555555555558</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>45485</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.80902777777777779</v>
+      </c>
       <c r="D17" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>45486</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="D18" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+        <v>0.20833333333333337</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D19" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D20" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D21" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D22" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D23" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D24" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D25" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D26" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D27" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D28" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D29" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D30" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D31" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D32" s="1">
         <f t="shared" si="1"/>
         <v>0</v>

</xml_diff>

<commit_message>
docs: 📝 finished textual content
</commit_message>
<xml_diff>
--- a/doc/journal_de_travail.xlsx
+++ b/doc/journal_de_travail.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TB\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4C4852-CCB5-4C7D-BA12-033C8F42754B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B7210C-0D9F-4B2D-AD80-6F0D0B469DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -395,7 +395,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,7 +429,7 @@
       </c>
       <c r="I1" s="3">
         <f>SUMIF(E:E, H1, D:D)</f>
-        <v>2.9430555555555555</v>
+        <v>3.229166666666667</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -572,7 +572,7 @@
       </c>
       <c r="I7" s="3">
         <f>SUM(I1:I5)</f>
-        <v>3.3180555555555555</v>
+        <v>3.604166666666667</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -792,9 +792,21 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>45488</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.95277777777777783</v>
+      </c>
       <c r="D20" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.2861111111111112</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
docs: 📝 migrated template
</commit_message>
<xml_diff>
--- a/doc/journal_de_travail.xlsx
+++ b/doc/journal_de_travail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TB\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B7210C-0D9F-4B2D-AD80-6F0D0B469DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C7BF9A-48C7-4197-9E42-4B5C2F99B216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4065" yWindow="3030" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -394,8 +394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,7 +429,7 @@
       </c>
       <c r="I1" s="3">
         <f>SUMIF(E:E, H1, D:D)</f>
-        <v>3.229166666666667</v>
+        <v>3.4368055555555559</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -572,7 +572,7 @@
       </c>
       <c r="I7" s="3">
         <f>SUM(I1:I5)</f>
-        <v>3.604166666666667</v>
+        <v>3.8118055555555559</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -810,9 +810,21 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>45490</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.99930555555555556</v>
+      </c>
       <c r="D21" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.20763888888888893</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
docs: 📝 added final version of report
</commit_message>
<xml_diff>
--- a/doc/journal_de_travail.xlsx
+++ b/doc/journal_de_travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TB\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C7BF9A-48C7-4197-9E42-4B5C2F99B216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F33CBCF-89EE-4A46-84AF-7265722C87A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4065" yWindow="3030" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -394,8 +394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,7 +429,7 @@
       </c>
       <c r="I1" s="3">
         <f>SUMIF(E:E, H1, D:D)</f>
-        <v>3.4368055555555559</v>
+        <v>3.6034722222222229</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -572,7 +572,7 @@
       </c>
       <c r="I7" s="3">
         <f>SUM(I1:I5)</f>
-        <v>3.8118055555555559</v>
+        <v>3.9784722222222229</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -828,15 +828,39 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>45491</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.5</v>
+      </c>
       <c r="D22" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8.3333333333333315E-2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>45492</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="D23" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8.3333333333333259E-2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat: ✨ added model training and export notebook
</commit_message>
<xml_diff>
--- a/doc/journal_de_travail.xlsx
+++ b/doc/journal_de_travail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TB\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F33CBCF-89EE-4A46-84AF-7265722C87A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C367BEB3-E56F-4D3B-9D76-D1776801E834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4065" yWindow="3030" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5505" yWindow="2220" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -394,8 +394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,7 +454,7 @@
       </c>
       <c r="I2" s="3">
         <f t="shared" ref="I2:I5" si="0">SUMIF(E:E, H2, D:D)</f>
-        <v>0</v>
+        <v>0.50000000000000011</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -572,7 +572,7 @@
       </c>
       <c r="I7" s="3">
         <f>SUM(I1:I5)</f>
-        <v>3.9784722222222229</v>
+        <v>4.4784722222222229</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -864,21 +864,57 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>45500</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.75</v>
+      </c>
       <c r="D24" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.16666666666666663</v>
+      </c>
+      <c r="E24" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>45512</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.57430555555555551</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.72569444444444453</v>
+      </c>
       <c r="D25" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.15138888888888902</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>45513</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.56805555555555554</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.75</v>
+      </c>
       <c r="D26" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.18194444444444446</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>